<commit_message>
nuts2 population prognosis now only takes into consideration the labels from nuts2_from_model.xlsx file
</commit_message>
<xml_diff>
--- a/output/endemo2_industry_coefficients_current_settings.xlsx
+++ b/output/endemo2_industry_coefficients_current_settings.xlsx
@@ -1939,7 +1939,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>(0, 0)</t>
+          <t>(2018.0, 0.0)</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -7022,10 +7022,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -7242,10 +7242,10 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
         <v>-0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -7286,10 +7286,10 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
         <v>-0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -7418,7 +7418,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>-0</v>
+        <v>-0.04</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -7682,7 +7682,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.01</v>
+        <v>-0</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -7726,7 +7726,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.01</v>
+        <v>-0</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -8022,7 +8022,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>(2018.0, 1.15645874983918e-05)</t>
+          <t>(2018.0, 1.1565663088379015e-05)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -8122,7 +8122,7 @@
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.01</v>
+        <v>-0</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -8511,7 +8511,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I4" t="n">
         <v>-0</v>
@@ -8643,7 +8643,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.01</v>
+        <v>-0.11</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -8687,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="I8" t="n">
         <v>-0</v>
@@ -8819,10 +8819,10 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.01</v>
+        <v>0.04</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -8863,7 +8863,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="I12" t="n">
         <v>-0</v>
@@ -8995,10 +8995,10 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="I15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -9171,7 +9171,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="I19" t="n">
         <v>-0</v>
@@ -9259,7 +9259,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="I21" t="n">
         <v>-0</v>
@@ -9435,10 +9435,10 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="I25" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
@@ -9523,7 +9523,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>-0</v>
@@ -9599,7 +9599,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>(2018.0, 0.00045155301091263385)</t>
+          <t>(2018.0, 0.0004515950085971429)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -9655,10 +9655,10 @@
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.09</v>
+        <v>0.02</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -9699,10 +9699,10 @@
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="I31" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -9831,7 +9831,7 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>-0</v>
+        <v>-0.02</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -11665,7 +11665,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>-0</v>
@@ -11753,10 +11753,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I6" t="n">
         <v>-0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -11929,7 +11929,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I10" t="n">
         <v>-0</v>
@@ -12017,10 +12017,10 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
         <v>-0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -12149,7 +12149,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>-0</v>
+        <v>-0.01</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -12281,7 +12281,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>-0</v>
+        <v>-0.02</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -12325,7 +12325,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -12753,7 +12753,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>(2018.0, 0.0001281741781071758)</t>
+          <t>(2018.0, 0.0001281860992295341)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -13330,10 +13330,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -13506,10 +13506,10 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -13990,10 +13990,10 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -19638,10 +19638,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
         <v>-0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -20034,7 +20034,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>-0</v>
+        <v>-0.01</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -20166,10 +20166,10 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I18" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>

</xml_diff>